<commit_message>
updated keyword with success close
</commit_message>
<xml_diff>
--- a/src/test/resources/key.xlsx
+++ b/src/test/resources/key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/53076bf53aa758bb/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="11_F25DC773A252ABDACC104875115E44585ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD1292D2-49C6-43F3-9A2D-099402AF7514}"/>
+  <xr:revisionPtr revIDLastSave="271" documentId="11_F25DC773A252ABDACC104875115E44585ADE58F5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5E47E281-D266-4174-9943-E39DDA2D2712}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,14 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>TestStep</t>
   </si>
   <si>
-    <t>Locator</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -75,19 +72,31 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>name=password</t>
-  </si>
-  <si>
     <t>http://localhost/opencart/upload/admin/</t>
   </si>
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t>name=username</t>
-  </si>
-  <si>
-    <t>xpath=/html/body/div/div[2]/div/div/div/div/div[2]/form/div[3]/button</t>
+    <t>LocatorName</t>
+  </si>
+  <si>
+    <t>LocatorValue</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>xpath</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>//button[@type='submit']</t>
   </si>
 </sst>
 </file>
@@ -483,249 +492,290 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="12.734375" customWidth="1"/>
-    <col min="2" max="2" width="29.15625" customWidth="1"/>
-    <col min="3" max="3" width="28.41796875" customWidth="1"/>
-    <col min="4" max="4" width="44" customWidth="1"/>
-    <col min="5" max="5" width="48.5234375" customWidth="1"/>
+    <col min="2" max="3" width="29.15625" customWidth="1"/>
+    <col min="4" max="4" width="28.41796875" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
+    <col min="6" max="6" width="48.5234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="3" t="s">
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="3" t="s">
+      <c r="F3" s="4"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="3" t="s">
+      <c r="E4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="3" t="s">
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" s="3"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>